<commit_message>
Optimize the Xlsx2Ifc generator for product libraries #41 * Added the IfcComplexProperties to the DataSheets für the DoP Library
</commit_message>
<xml_diff>
--- a/SampleFiles/DoPLibrary/SourceData/BaustoffindustrieTemplatesAndSheets.xlsx
+++ b/SampleFiles/DoPLibrary/SourceData/BaustoffindustrieTemplatesAndSheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\buildingSMART\ProductData\SampleFiles\DoPLibrary\SourceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F51717F-FD97-4240-BD6B-D721CD58F800}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D265F7-4492-48D0-B100-B4369933A61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="396" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Templates" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="310">
   <si>
     <t>SystemName</t>
   </si>
@@ -1051,6 +1051,9 @@
   </si>
   <si>
     <t>Value1|Value2|Value3|NPD</t>
+  </si>
+  <si>
+    <t>DoP data template according to EN 771-5 (Test)</t>
   </si>
 </sst>
 </file>
@@ -1305,25 +1308,6 @@
   </cellStyles>
   <dxfs count="73">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1381,6 +1365,25 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
@@ -2511,14 +2514,14 @@
     <tableColumn id="45" xr3:uid="{C8FEB31C-E786-439C-9EF6-D7C6EDB36D4E}" name="Leistung zu 9.108" dataDxfId="10"/>
     <tableColumn id="46" xr3:uid="{7DA426C6-F04F-462F-8E8F-5073B0845291}" name="Leistung zu 9.109" dataDxfId="9"/>
     <tableColumn id="47" xr3:uid="{C45B615C-C96C-4883-98A9-2825C74413E1}" name="Leistung zu 9.110" dataDxfId="8"/>
-    <tableColumn id="48" xr3:uid="{7A08FC86-461E-4D43-B179-673D163C4086}" name="Leistung zu 9.111" dataDxfId="0"/>
-    <tableColumn id="60" xr3:uid="{1B428CD1-B942-4A1D-ACBE-1C037EE4EF4E}" name="Harmonisierte technische Spezifikation" dataDxfId="7" dataCellStyle="Standard 2"/>
-    <tableColumn id="61" xr3:uid="{79E50F33-F59A-4A05-8902-22640B19B8E2}" name="Name, Funktion" dataDxfId="6"/>
-    <tableColumn id="62" xr3:uid="{6B4AC729-A672-46C0-9393-64E19C5BBE95}" name="Ort und Datum" dataDxfId="5"/>
-    <tableColumn id="63" xr3:uid="{03A3A100-F48E-4BCD-BC7C-1A0F3A675C39}" name="Unterschrift" dataDxfId="4"/>
-    <tableColumn id="64" xr3:uid="{DE5DE9CF-2ECB-4520-90F1-D7BB0934C878}" name="Dokumentenreferenzierung/ProductDataSheet" dataDxfId="3"/>
-    <tableColumn id="65" xr3:uid="{DAA38489-BC36-4FC1-8105-47753E5BF89F}" name="Omniclass" dataDxfId="2"/>
-    <tableColumn id="66" xr3:uid="{7D636AEA-8665-43B5-B305-974C6190537C}" name="Uniclass" dataDxfId="1"/>
+    <tableColumn id="48" xr3:uid="{7A08FC86-461E-4D43-B179-673D163C4086}" name="Leistung zu 9.111" dataDxfId="7"/>
+    <tableColumn id="60" xr3:uid="{1B428CD1-B942-4A1D-ACBE-1C037EE4EF4E}" name="Harmonisierte technische Spezifikation" dataDxfId="6" dataCellStyle="Standard 2"/>
+    <tableColumn id="61" xr3:uid="{79E50F33-F59A-4A05-8902-22640B19B8E2}" name="Name, Funktion" dataDxfId="5"/>
+    <tableColumn id="62" xr3:uid="{6B4AC729-A672-46C0-9393-64E19C5BBE95}" name="Ort und Datum" dataDxfId="4"/>
+    <tableColumn id="63" xr3:uid="{03A3A100-F48E-4BCD-BC7C-1A0F3A675C39}" name="Unterschrift" dataDxfId="3"/>
+    <tableColumn id="64" xr3:uid="{DE5DE9CF-2ECB-4520-90F1-D7BB0934C878}" name="Dokumentenreferenzierung/ProductDataSheet" dataDxfId="2"/>
+    <tableColumn id="65" xr3:uid="{DAA38489-BC36-4FC1-8105-47753E5BF89F}" name="Omniclass" dataDxfId="1"/>
+    <tableColumn id="66" xr3:uid="{7D636AEA-8665-43B5-B305-974C6190537C}" name="Uniclass" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2789,28 +2792,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A07687-0D17-4D6E-8F6E-1C562F7CF42C}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="13" customWidth="1"/>
-    <col min="2" max="4" width="20.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" style="13" customWidth="1"/>
-    <col min="10" max="13" width="22.33203125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="41.5546875" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="11.5546875" style="13"/>
+    <col min="1" max="1" width="17.28515625" style="13" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" style="13" customWidth="1"/>
+    <col min="10" max="13" width="22.28515625" style="13" customWidth="1"/>
+    <col min="14" max="14" width="41.5703125" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="11.5703125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>216</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>216</v>
       </c>
@@ -2900,7 +2903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>216</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>216</v>
       </c>
@@ -2949,7 +2952,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>216</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>216</v>
       </c>
@@ -2995,7 +2998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>216</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>216</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>216</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>216</v>
       </c>
@@ -3087,7 +3090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>216</v>
       </c>
@@ -3110,7 +3113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>216</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>216</v>
       </c>
@@ -3156,7 +3159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>216</v>
       </c>
@@ -3179,7 +3182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>216</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>216</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>216</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>216</v>
       </c>
@@ -3271,7 +3274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>216</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>216</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>216</v>
       </c>
@@ -3340,7 +3343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>216</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>216</v>
       </c>
@@ -3401,7 +3404,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>216</v>
       </c>
@@ -3442,7 +3445,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>216</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>216</v>
       </c>
@@ -3524,7 +3527,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>216</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>216</v>
       </c>
@@ -3570,7 +3573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>216</v>
       </c>
@@ -3595,7 +3598,7 @@
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
     </row>
-    <row r="31" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>216</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>216</v>
       </c>
@@ -3644,7 +3647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>216</v>
       </c>
@@ -3667,7 +3670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>216</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>216</v>
       </c>
@@ -3713,7 +3716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>216</v>
       </c>
@@ -3736,7 +3739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>216</v>
       </c>
@@ -3759,12 +3762,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>109</v>
@@ -3782,12 +3785,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>110</v>
@@ -3805,12 +3808,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>111</v>
@@ -3828,12 +3831,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>112</v>
@@ -3851,12 +3854,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F42" s="14" t="s">
         <v>113</v>
@@ -3874,12 +3877,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>114</v>
@@ -3897,12 +3900,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>115</v>
@@ -3920,12 +3923,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>116</v>
@@ -3943,12 +3946,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>117</v>
@@ -3966,12 +3969,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>119</v>
@@ -3989,12 +3992,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>121</v>
@@ -4012,7 +4015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>216</v>
       </c>
@@ -4038,7 +4041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>216</v>
       </c>
@@ -4064,7 +4067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
         <v>216</v>
       </c>
@@ -4090,7 +4093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
         <v>216</v>
       </c>
@@ -4116,7 +4119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>216</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>216</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>216</v>
       </c>
@@ -4193,48 +4196,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD445CDE-C2A4-4DDD-ACCB-5C973BA54256}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" style="33" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="57.109375" style="33" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="49.44140625" style="33" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" style="33" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" style="33" customWidth="1"/>
-    <col min="9" max="12" width="50.6640625" style="33" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" style="33" customWidth="1"/>
-    <col min="14" max="14" width="50.6640625" style="33" customWidth="1"/>
-    <col min="15" max="15" width="51.6640625" style="33" customWidth="1"/>
-    <col min="16" max="17" width="17.33203125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="33" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" style="33" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" style="33" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="33" customWidth="1"/>
+    <col min="9" max="12" width="50.7109375" style="33" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" style="33" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" style="33" customWidth="1"/>
+    <col min="15" max="15" width="51.7109375" style="33" customWidth="1"/>
+    <col min="16" max="17" width="17.28515625" style="33" customWidth="1"/>
     <col min="18" max="18" width="23" style="33" customWidth="1"/>
     <col min="19" max="19" width="41" style="33" customWidth="1"/>
-    <col min="20" max="20" width="45.33203125" style="33" customWidth="1"/>
-    <col min="21" max="21" width="57.109375" style="33" customWidth="1"/>
-    <col min="22" max="22" width="46.33203125" style="33" customWidth="1"/>
-    <col min="23" max="23" width="57.109375" style="33" customWidth="1"/>
-    <col min="24" max="24" width="47.6640625" style="33" customWidth="1"/>
-    <col min="25" max="25" width="21.33203125" style="33" customWidth="1"/>
-    <col min="26" max="26" width="23.33203125" style="33" customWidth="1"/>
-    <col min="27" max="27" width="29.5546875" style="33" customWidth="1"/>
-    <col min="28" max="35" width="22.6640625" style="33" customWidth="1"/>
-    <col min="36" max="37" width="23.6640625" style="33" customWidth="1"/>
-    <col min="38" max="48" width="17.33203125" style="33" customWidth="1"/>
+    <col min="20" max="20" width="45.28515625" style="33" customWidth="1"/>
+    <col min="21" max="21" width="57.140625" style="33" customWidth="1"/>
+    <col min="22" max="22" width="46.28515625" style="33" customWidth="1"/>
+    <col min="23" max="23" width="57.140625" style="33" customWidth="1"/>
+    <col min="24" max="24" width="47.7109375" style="33" customWidth="1"/>
+    <col min="25" max="25" width="21.28515625" style="33" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="33" customWidth="1"/>
+    <col min="27" max="27" width="29.5703125" style="33" customWidth="1"/>
+    <col min="28" max="35" width="22.7109375" style="33" customWidth="1"/>
+    <col min="36" max="37" width="23.7109375" style="33" customWidth="1"/>
+    <col min="38" max="48" width="17.28515625" style="33" customWidth="1"/>
     <col min="49" max="55" width="16" style="33" customWidth="1"/>
-    <col min="56" max="56" width="34.33203125" style="33" customWidth="1"/>
-    <col min="57" max="57" width="15.5546875" style="33" customWidth="1"/>
-    <col min="58" max="58" width="14.6640625" style="33" customWidth="1"/>
-    <col min="59" max="59" width="12.33203125" style="33" customWidth="1"/>
-    <col min="60" max="60" width="42.44140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="61" max="16384" width="11.44140625" style="33"/>
+    <col min="56" max="56" width="34.28515625" style="33" customWidth="1"/>
+    <col min="57" max="57" width="15.5703125" style="33" customWidth="1"/>
+    <col min="58" max="58" width="14.7109375" style="33" customWidth="1"/>
+    <col min="59" max="59" width="12.28515625" style="33" customWidth="1"/>
+    <col min="60" max="60" width="42.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="61" max="16384" width="11.42578125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="26" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" s="26" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>283</v>
       </c>
@@ -4401,7 +4404,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>78</v>
       </c>
@@ -4559,7 +4562,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>79</v>
       </c>
@@ -4717,7 +4720,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>80</v>
       </c>
@@ -4875,7 +4878,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>77</v>
       </c>
@@ -5031,7 +5034,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="96" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" ht="92.25" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>141</v>
       </c>
@@ -5210,19 +5213,19 @@
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.88671875" style="2"/>
+    <col min="2" max="2" width="62.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="5" t="s">
@@ -5241,7 +5244,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -5264,7 +5267,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -5287,7 +5290,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -5307,7 +5310,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -5330,7 +5333,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -5353,7 +5356,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -5376,7 +5379,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -5399,7 +5402,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -5422,7 +5425,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -5468,7 +5471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -5491,7 +5494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
@@ -5510,7 +5513,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -5529,7 +5532,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
@@ -5548,7 +5551,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
@@ -5567,7 +5570,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -5586,7 +5589,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
@@ -5605,7 +5608,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>204</v>
       </c>
@@ -5618,7 +5621,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>205</v>
       </c>
@@ -5631,7 +5634,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>206</v>
       </c>
@@ -5644,7 +5647,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>207</v>
       </c>
@@ -5657,7 +5660,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>208</v>
       </c>
@@ -5670,7 +5673,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>85</v>
       </c>
@@ -5693,7 +5696,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>86</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>87</v>
       </c>
@@ -5739,7 +5742,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>88</v>
       </c>
@@ -5762,7 +5765,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>89</v>
       </c>
@@ -5785,7 +5788,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>90</v>
       </c>
@@ -5808,7 +5811,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>91</v>
       </c>
@@ -5831,7 +5834,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>92</v>
       </c>
@@ -5854,7 +5857,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>93</v>
       </c>
@@ -5877,7 +5880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>103</v>
       </c>
@@ -5900,7 +5903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>104</v>
       </c>
@@ -5923,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>94</v>
       </c>
@@ -5946,7 +5949,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>95</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>96</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>97</v>
       </c>
@@ -6015,7 +6018,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>98</v>
       </c>
@@ -6038,7 +6041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>99</v>
       </c>
@@ -6061,7 +6064,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
@@ -6084,7 +6087,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>101</v>
       </c>
@@ -6107,7 +6110,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>102</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>118</v>
       </c>
@@ -6153,7 +6156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>120</v>
       </c>
@@ -6176,7 +6179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>156</v>
       </c>
@@ -6199,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>157</v>
       </c>
@@ -6222,7 +6225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>158</v>
       </c>
@@ -6245,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>159</v>
       </c>
@@ -6268,7 +6271,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>160</v>
       </c>
@@ -6291,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>161</v>
       </c>
@@ -6314,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>162</v>
       </c>
@@ -6337,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>163</v>
       </c>
@@ -6360,7 +6363,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>164</v>
       </c>
@@ -6383,7 +6386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>165</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>166</v>
       </c>
@@ -6429,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>45</v>
       </c>
@@ -6452,7 +6455,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>26</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>27</v>
       </c>
@@ -6498,7 +6501,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>28</v>
       </c>
@@ -6511,7 +6514,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>29</v>
       </c>

</xml_diff>